<commit_message>
[Pat, Minno] #203 app can now parse excel files through column name.
</commit_message>
<xml_diff>
--- a/src/main/ruby/Test.xlsx
+++ b/src/main/ruby/Test.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="34400" windowHeight="20940" tabRatio="500"/>
+    <workbookView xWindow="18340" yWindow="540" windowWidth="17680" windowHeight="10860" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="happy-path" sheetId="1" r:id="rId1"/>
+    <sheet name="offset-columns" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="130404"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
@@ -77,6 +77,34 @@
   </si>
   <si>
     <t>15/10/2004</t>
+  </si>
+  <si>
+    <t>I offset the rest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*muahahaha*</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Minno</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Female</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blub</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Blab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>25/12/1999</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -186,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -198,9 +226,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -223,11 +248,20 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,7 +594,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -581,108 +615,108 @@
       <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" ht="23">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="7"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="15">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9" t="s">
+      <c r="E4" s="17"/>
+      <c r="F4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="10" t="s">
+      <c r="G4" s="17"/>
+      <c r="H4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="11"/>
+      <c r="J4" s="10"/>
     </row>
     <row r="5" spans="1:10" ht="16">
-      <c r="A5" s="12">
+      <c r="A5" s="11">
         <v>1</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14" t="s">
+      <c r="E5" s="15"/>
+      <c r="F5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="13" t="s">
+      <c r="G5" s="15"/>
+      <c r="H5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="16"/>
+      <c r="J5" s="14"/>
     </row>
     <row r="6" spans="1:10" ht="16">
-      <c r="A6" s="12">
+      <c r="A6" s="11">
         <v>2</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14" t="s">
+      <c r="E6" s="15"/>
+      <c r="F6" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="13" t="s">
+      <c r="G6" s="15"/>
+      <c r="H6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="12">
         <v>9916707349</v>
       </c>
-      <c r="J6" s="16"/>
+      <c r="J6" s="14"/>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
@@ -697,7 +731,6 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" scale="71" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="28" max="16383" man="1"/>
   </rowBreaks>
@@ -715,19 +748,136 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="16">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" ht="23">
+      <c r="A2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" ht="18">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:11" ht="15">
+      <c r="A4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="17"/>
+      <c r="I4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="10"/>
+    </row>
+    <row r="5" spans="1:11" ht="16">
+      <c r="A5" s="11">
+        <v>1</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="15"/>
+      <c r="I5" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="13"/>
+      <c r="K5" s="14"/>
+    </row>
+  </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
+  <mergeCells count="5">
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="27" max="16383" man="1"/>
+  </rowBreaks>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="10" max="1048575" man="1"/>
+  </colBreaks>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>